<commit_message>
Nickname importer should now grab nicknames for the proper classes.
</commit_message>
<xml_diff>
--- a/Xcom2ClassManager/XComAbilityList.xlsx
+++ b/Xcom2ClassManager/XComAbilityList.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="1136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="1146">
   <si>
     <t>Name</t>
   </si>
@@ -3427,6 +3427,36 @@
   </si>
   <si>
     <t>Gain &lt;Ability:+Crit/&gt; Crit chance and &lt;Ability:+Mobility/&gt; Mobility while equipped with a shotgun.</t>
+  </si>
+  <si>
+    <t>DoubleTap2</t>
+  </si>
+  <si>
+    <t>Activate to fire a standard shot and gain a second action restricted to an additional shot or overwatching.</t>
+  </si>
+  <si>
+    <t>QuickStudy</t>
+  </si>
+  <si>
+    <t>Quick Study</t>
+  </si>
+  <si>
+    <t>Learn officer and AWC bonus abilities in half the time.</t>
+  </si>
+  <si>
+    <t>RescueProtocol</t>
+  </si>
+  <si>
+    <t>Rescue Protocol</t>
+  </si>
+  <si>
+    <t>Use your Gremlin to grant a movement action to an ally.</t>
+  </si>
+  <si>
+    <t>Solace_LW</t>
+  </si>
+  <si>
+    <t>The Psi Operative may immediately extinguish mental impairments for a squadmate.</t>
   </si>
 </sst>
 </file>
@@ -3769,7 +3799,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G388"/>
+  <dimension ref="A1:G392"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
       <selection activeCell="F76" sqref="F76"/>
@@ -10598,6 +10628,74 @@
       </c>
       <c r="E388" s="0" t="s">
         <v>793</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" s="0" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B389" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="C389" s="0" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D389" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E389" s="0" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" s="0" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B390" s="0" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C390" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D390" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E390" s="0" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" s="0" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B391" s="0" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C391" s="0" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D391" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E391" s="0" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" s="0" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B392" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="C392" s="0" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D392" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E392" s="0" t="s">
+        <v>259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weapons now use a list view. Import abilities for has larger description text box.
</commit_message>
<xml_diff>
--- a/Xcom2ClassManager/XComAbilityList.xlsx
+++ b/Xcom2ClassManager/XComAbilityList.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="1146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="1417">
   <si>
     <t>Name</t>
   </si>
@@ -3457,6 +3457,819 @@
   </si>
   <si>
     <t>The Psi Operative may immediately extinguish mental impairments for a squadmate.</t>
+  </si>
+  <si>
+    <t>TankLW2AbsorptionField</t>
+  </si>
+  <si>
+    <t>Absorption Field</t>
+  </si>
+  <si>
+    <t>The unit is surrounded by a damage absorbing field that immediately lowers incoming damage for the unit itself and any allies inside the field.</t>
+  </si>
+  <si>
+    <t>LW2 Tank</t>
+  </si>
+  <si>
+    <t>TankLW2AdvancedStorage</t>
+  </si>
+  <si>
+    <t>Advanced Storage</t>
+  </si>
+  <si>
+    <t>You can use PROTECTION PROTOCOL also on other units.</t>
+  </si>
+  <si>
+    <t>TankLW2BallisticVests</t>
+  </si>
+  <si>
+    <t>Ballistic Vests</t>
+  </si>
+  <si>
+    <t>Gain +1 extra point of armor for each vest or plating you equipp on this soldier.</t>
+  </si>
+  <si>
+    <t>TankLW2Challenge</t>
+  </si>
+  <si>
+    <t>Challenge</t>
+  </si>
+  <si>
+    <t>Challenge a target and make it to your main enemy. Soldiers with this ability gain bonuses when attacking the challenged target. Soldiers with this ability are motivating themselves and nearby allies temporarily, if the challenged enemy was killed.</t>
+  </si>
+  <si>
+    <t>TankLW2CombatDrugs</t>
+  </si>
+  <si>
+    <t>Grants 1 free overdrive serum item to your inventory.</t>
+  </si>
+  <si>
+    <t>TankLW2Decoy</t>
+  </si>
+  <si>
+    <t>Decoy</t>
+  </si>
+  <si>
+    <t>Grants 1 free mimic beacon item to your inventory.</t>
+  </si>
+  <si>
+    <t>TankLW2EverSafe</t>
+  </si>
+  <si>
+    <t>Ever Safe</t>
+  </si>
+  <si>
+    <t>If you spend all of your actions on moves, you are granted an automatic PROTECTION PROTOCOL at the end of the turn.</t>
+  </si>
+  <si>
+    <t>TankLW2HereIAm</t>
+  </si>
+  <si>
+    <t>Here I Am</t>
+  </si>
+  <si>
+    <t>Try to make this soldier a main target. Attacks against this unit gain +60% aim chance, but suffer a -20% penalty to critical hit chances for one turn. Warning: probably garanteed to hit.</t>
+  </si>
+  <si>
+    <t>TankLW2LastChance</t>
+  </si>
+  <si>
+    <t>Nano Stabilizer</t>
+  </si>
+  <si>
+    <t>Once per Mission, if the tank takes lethal damage, instead of dying, the tanklin immediately activates PROTECTION PROTOCOL and heals the unit to 5 HP.</t>
+  </si>
+  <si>
+    <t>TankLW2PreFire</t>
+  </si>
+  <si>
+    <t>Pre Fire</t>
+  </si>
+  <si>
+    <t>When targeted by enemy fire, automatically fire a preemptive reaction shot with your primary weapon once per turn.</t>
+  </si>
+  <si>
+    <t>TankLW2ProtectionProtocolAblative</t>
+  </si>
+  <si>
+    <t>Protection Protocol</t>
+  </si>
+  <si>
+    <t>Command your tanklin to activate an energy shield. It grants the target different defensive bonuses.</t>
+  </si>
+  <si>
+    <t>TankLW2ReflectionField</t>
+  </si>
+  <si>
+    <t>Reflection Field</t>
+  </si>
+  <si>
+    <t>The unit is surrounded by a reflecting field. Any incoming damage from shots has a 25% chance to become reflected instead of hiting the unit.</t>
+  </si>
+  <si>
+    <t>TankLW2Revenge</t>
+  </si>
+  <si>
+    <t>Revenge</t>
+  </si>
+  <si>
+    <t>When targeted by enemy fire, automatically fire back with your primary weapon once per turn.</t>
+  </si>
+  <si>
+    <t>TankLW2ShieldHit</t>
+  </si>
+  <si>
+    <t>Self Defense Uplink</t>
+  </si>
+  <si>
+    <t>Tanks gain free melee attacks on any enemies that enter or attack from melee range as long as PROTECTION PROTOCOL is active.</t>
+  </si>
+  <si>
+    <t>TankLW2ShockAbsorbantArmor</t>
+  </si>
+  <si>
+    <t>Shock Absorbant Armor</t>
+  </si>
+  <si>
+    <t>Damage received within 2 tiles radius is reduced.</t>
+  </si>
+  <si>
+    <t>TankLW2StandBy</t>
+  </si>
+  <si>
+    <t>Standby</t>
+  </si>
+  <si>
+    <t>All reaction hits of this soldier can critically hit. The unit also has +10% aim and +10% crit chance as well as +1 additional base damage on all reaction shots and other reflex abilities.</t>
+  </si>
+  <si>
+    <t>TankLW2Steadfast</t>
+  </si>
+  <si>
+    <t>Steadfast</t>
+  </si>
+  <si>
+    <t>Never panic as a result of getting wounded, or allies getting killed. Also gain immunity to stun.</t>
+  </si>
+  <si>
+    <t>TankLW2SurvivalTraining</t>
+  </si>
+  <si>
+    <t>Survival Training</t>
+  </si>
+  <si>
+    <t>Heal immediatly +5 HP, fire, acid, poison and hunker down. Also reduces wound recovery time for this unit significantly.</t>
+  </si>
+  <si>
+    <t>TankLW2Suspension</t>
+  </si>
+  <si>
+    <t>Suspension</t>
+  </si>
+  <si>
+    <t>Incoming damage from reaction attacks is reduced.</t>
+  </si>
+  <si>
+    <t>TankLW2TeamShield</t>
+  </si>
+  <si>
+    <t>Team Shield</t>
+  </si>
+  <si>
+    <t>Activate an area of effect energy shield. It grants this unit and teammates ablative HP.</t>
+  </si>
+  <si>
+    <t>TankLW2WarningShot</t>
+  </si>
+  <si>
+    <t>Warning Shot</t>
+  </si>
+  <si>
+    <t>A special shot with a high chance to apply panic on your target, whether or not it hits or misses but a successful hit will only graze the target.</t>
+  </si>
+  <si>
+    <t>Op_BoundingFire</t>
+  </si>
+  <si>
+    <t>Bounding Fire</t>
+  </si>
+  <si>
+    <t>Any shot taken as your second action after moving as your first confers a +10 aim bonus.</t>
+  </si>
+  <si>
+    <t>LW2 Operator</t>
+  </si>
+  <si>
+    <t>Op_BreachAndClear</t>
+  </si>
+  <si>
+    <t>Flash Out</t>
+  </si>
+  <si>
+    <t>Activate this ability before throwing or launching a flashbang grenade, and the throw will not cost an action.</t>
+  </si>
+  <si>
+    <t>Op_Ghost</t>
+  </si>
+  <si>
+    <t>Ghost</t>
+  </si>
+  <si>
+    <t>While concealed, enemy detection range against this unit is half that of a normal soldier.</t>
+  </si>
+  <si>
+    <t>Op_HardYards</t>
+  </si>
+  <si>
+    <t>Hard Yards</t>
+  </si>
+  <si>
+    <t>Activate this ability to shrug off 75% of reaction fire damage for the rest of your turn. 2 turn cooldown.</t>
+  </si>
+  <si>
+    <t>Op_HiddenKiller</t>
+  </si>
+  <si>
+    <t>Hidden Killer</t>
+  </si>
+  <si>
+    <t>While concealed or flanking your target, you deal +2 damage with your primary weapon. Passive.</t>
+  </si>
+  <si>
+    <t>Op_HoldPosition</t>
+  </si>
+  <si>
+    <t>Hold Position</t>
+  </si>
+  <si>
+    <t>From full cover take a reaction shot against any enemy that moves or attacks within your vision until you run out of ammo. 4 turn cooldown.</t>
+  </si>
+  <si>
+    <t>Op_LethalForce</t>
+  </si>
+  <si>
+    <t>Lethal Force</t>
+  </si>
+  <si>
+    <t>You do two additional points of base damage with your primary weapon to targets within 8 tiles. Passive.</t>
+  </si>
+  <si>
+    <t>Op_NoPrisoners</t>
+  </si>
+  <si>
+    <t>No Prisoners</t>
+  </si>
+  <si>
+    <t>You deal an additional +2 damage to stunned or disorientated enemies with your primary weapon.</t>
+  </si>
+  <si>
+    <t>Op_Raptor</t>
+  </si>
+  <si>
+    <t>Raptor</t>
+  </si>
+  <si>
+    <t>You get an additional +25 Crit chance against targets at a lower elevation. Passive.</t>
+  </si>
+  <si>
+    <t>Op_Sentry</t>
+  </si>
+  <si>
+    <t>Sentry</t>
+  </si>
+  <si>
+    <t>Grants +10 Aim and Covering Fire on Overwatch and allows overwatch shots to do critical damage. Passive.</t>
+  </si>
+  <si>
+    <t>Op_SettledShot</t>
+  </si>
+  <si>
+    <t>Settled Shot</t>
+  </si>
+  <si>
+    <t>Special shot that requires both action points but has a +25 crit chance and deals +3 damage on succesful critical hits. 2 turn cooldown.</t>
+  </si>
+  <si>
+    <t>Op_Stalker</t>
+  </si>
+  <si>
+    <t>Wraith</t>
+  </si>
+  <si>
+    <t>Whenever you kill an enemy, critical hits will restore concealment.</t>
+  </si>
+  <si>
+    <t>Op_StealthShot</t>
+  </si>
+  <si>
+    <t>Stealth Shot</t>
+  </si>
+  <si>
+    <t>Fire a shot whilst concealed with a +50 crit chance bonus. If you kill your target maintain concealment. 5 turn cooldown.</t>
+  </si>
+  <si>
+    <t>Op_TargetDown</t>
+  </si>
+  <si>
+    <t>Breach And Clear</t>
+  </si>
+  <si>
+    <t>When this ability is activated your actions will be refunded each time a stunned or disorientated enemy is killed. 4 turn cooldown.</t>
+  </si>
+  <si>
+    <t>Op_TargetDown2</t>
+  </si>
+  <si>
+    <t>Target Down</t>
+  </si>
+  <si>
+    <t>When you get a kill, you gain +20 defence until the end of the next alien turn. Passive.</t>
+  </si>
+  <si>
+    <t>Op_Wraith</t>
+  </si>
+  <si>
+    <t>Shadow</t>
+  </si>
+  <si>
+    <t>Gain +3 Mobility and +10 Aim while concealed. Passive.</t>
+  </si>
+  <si>
+    <t>TF_Ambush</t>
+  </si>
+  <si>
+    <t>Ambush Expert</t>
+  </si>
+  <si>
+    <t>Activate this ability to reduce enemy detection range against you by 60% for the rest of your turn. Five-turn cooldown.</t>
+  </si>
+  <si>
+    <t>LW2 Jackal</t>
+  </si>
+  <si>
+    <t>TF_Assassin</t>
+  </si>
+  <si>
+    <t>When you kill a flanked or uncovered enemy with your primary weapon, you gain concealment.</t>
+  </si>
+  <si>
+    <t>TF_BulletShred</t>
+  </si>
+  <si>
+    <t>Shatter Cartridges</t>
+  </si>
+  <si>
+    <t>A ferocious sawed-off shotgun attack dealing critical damage and ensuring that the target takes an additional +3 damage from all attacks in the future. Uses 2 ammo and has a 3 turn cooldown.</t>
+  </si>
+  <si>
+    <t>TF_CrowdControl</t>
+  </si>
+  <si>
+    <t>Crowd Control</t>
+  </si>
+  <si>
+    <t>Special shot for sawed-off shotguns only: Fire a short-range cone-based attack at nearby targets. Three-turn cooldown.</t>
+  </si>
+  <si>
+    <t>TF_GraphitePlates</t>
+  </si>
+  <si>
+    <t>Heavy Infantry</t>
+  </si>
+  <si>
+    <t>The Jackal is outfitted with graphite armour plates gaining +2 Armor at the expense of -1 mobility.</t>
+  </si>
+  <si>
+    <t>TF_HardYards</t>
+  </si>
+  <si>
+    <t>Activate this ability to allow the Jackal to shrug off reaction fire for half damage for the rest of your turn. 2 turn cooldown.</t>
+  </si>
+  <si>
+    <t>TF_HipFire</t>
+  </si>
+  <si>
+    <t>A free shot with your primary weapon at a small penalty to aim. 3 Turn Cooldown.</t>
+  </si>
+  <si>
+    <t>TF_LethalForce</t>
+  </si>
+  <si>
+    <t>You do two additional points of base damage with your primary weapon to targets within 8 tiles.</t>
+  </si>
+  <si>
+    <t>TF_Opportunist</t>
+  </si>
+  <si>
+    <t>You get an additional +10 to aim and +20 Crit chance against flanked targets.</t>
+  </si>
+  <si>
+    <t>TF_Ruthless</t>
+  </si>
+  <si>
+    <t>Ruthless</t>
+  </si>
+  <si>
+    <t>Your sawed-off shotgun attacks are significantly more accurate.</t>
+  </si>
+  <si>
+    <t>TF_StayingPower</t>
+  </si>
+  <si>
+    <t>Staying Power</t>
+  </si>
+  <si>
+    <t>Permanently gain 4 HP and 20 will.</t>
+  </si>
+  <si>
+    <t>TF_Tempest</t>
+  </si>
+  <si>
+    <t>Tempest</t>
+  </si>
+  <si>
+    <t>The Jackal fires their weapon at every visible enemy within 10 tiles. 4 turn cooldown, 2 ammo cost.</t>
+  </si>
+  <si>
+    <t>Op_AgainstTheOdds</t>
+  </si>
+  <si>
+    <t>Gain +3 Aim per enemy the squad can see up to a maximum of +15.</t>
+  </si>
+  <si>
+    <t>LW2 Jaegar</t>
+  </si>
+  <si>
+    <t>Op_Brutestrength</t>
+  </si>
+  <si>
+    <t>Brute Strength</t>
+  </si>
+  <si>
+    <t>All melee attacks deal +2 extra damage and have +10 Aim.</t>
+  </si>
+  <si>
+    <t>Op_HeadShot</t>
+  </si>
+  <si>
+    <t>Headshot</t>
+  </si>
+  <si>
+    <t>Special shot that has +100 crit chance and deals +5 damage on crit. 4 Turn cooldown.</t>
+  </si>
+  <si>
+    <t>Op_Marksman</t>
+  </si>
+  <si>
+    <t>Designated Marksman</t>
+  </si>
+  <si>
+    <t>You get +20 Aim against targets in full cover.</t>
+  </si>
+  <si>
+    <t>Op_Mountaineer</t>
+  </si>
+  <si>
+    <t>Mountaineer</t>
+  </si>
+  <si>
+    <t>You get an additional +10 Defense against targets at lower elevation.</t>
+  </si>
+  <si>
+    <t>Op_Pointman</t>
+  </si>
+  <si>
+    <t>First Contact</t>
+  </si>
+  <si>
+    <t>Each time an enemy is revealed there is a 25% chance to take a free overwatch shot as long as you have enough ammo. Will trigger once per enemy.</t>
+  </si>
+  <si>
+    <t>Op_QuickTarget</t>
+  </si>
+  <si>
+    <t>Lookout</t>
+  </si>
+  <si>
+    <t>Increase the chance of First Contact triggering on each revealed enemy from 25% to 50%.</t>
+  </si>
+  <si>
+    <t>Op_Skirmisher</t>
+  </si>
+  <si>
+    <t>Op_Spearhead</t>
+  </si>
+  <si>
+    <t>Spearhead</t>
+  </si>
+  <si>
+    <t>Gain 25% bonus damage against enemies who are hit by First Contact fire.</t>
+  </si>
+  <si>
+    <t>Op_Stamina</t>
+  </si>
+  <si>
+    <t>Stamina</t>
+  </si>
+  <si>
+    <t>Intense conditioning confers +3 mobility.</t>
+  </si>
+  <si>
+    <t>Op_Tempest</t>
+  </si>
+  <si>
+    <t>Tempest Fire</t>
+  </si>
+  <si>
+    <t>Fire your weapon at every visible enemy within 10 tiles. 4 turn cooldown, 3 ammo cost.</t>
+  </si>
+  <si>
+    <t>Op_TwistTheBlade</t>
+  </si>
+  <si>
+    <t>Twist the Blade</t>
+  </si>
+  <si>
+    <t>A ferocious melee attack dealing critical damage and ensuring that the target takes an additional +3 damage from all attacks in the future.</t>
+  </si>
+  <si>
+    <t>Lucu_Sniper_BallisticsExpert</t>
+  </si>
+  <si>
+    <t>Ballistics Expert</t>
+  </si>
+  <si>
+    <t>Reduced aim penalties for Squadsight at long ranges.</t>
+  </si>
+  <si>
+    <t>Lucubration's Sniper Class</t>
+  </si>
+  <si>
+    <t>Lucu_Sniper_CoverTarget</t>
+  </si>
+  <si>
+    <t>Cover Target</t>
+  </si>
+  <si>
+    <t>Overwatch a single target with Covering Fire. This attack may critically hit.</t>
+  </si>
+  <si>
+    <t>Lucu_Sniper_FollowUp</t>
+  </si>
+  <si>
+    <t>Follow-Up</t>
+  </si>
+  <si>
+    <t>Once per turn, if you hit with an attack but do not kill your target, you gain a bonus Follow-Up attack against the same target.</t>
+  </si>
+  <si>
+    <t>Lucu_Sniper_Hide</t>
+  </si>
+  <si>
+    <t>Hide</t>
+  </si>
+  <si>
+    <t>While Set Up, you may enter concealment if you did not attack last turn. This concealment is lost if you move or attack. Your attacks from concealment gain +20 crit.</t>
+  </si>
+  <si>
+    <t>Lucu_Sniper_InTheZone</t>
+  </si>
+  <si>
+    <t>In the Zone</t>
+  </si>
+  <si>
+    <t>Killing a flanked or uncovered target grants 1 bonus attack.</t>
+  </si>
+  <si>
+    <t>Lucu_Sniper_LowProfile</t>
+  </si>
+  <si>
+    <t>Treat low cover as high cover.</t>
+  </si>
+  <si>
+    <t>Lucu_Sniper_PrecisionShot</t>
+  </si>
+  <si>
+    <t>Fire a shot that does +1/+2/+3 damage and has +30 crit. 2 turn cooldown.</t>
+  </si>
+  <si>
+    <t>Lucu_Sniper_Relocation</t>
+  </si>
+  <si>
+    <t>Relocation</t>
+  </si>
+  <si>
+    <t>Once per turn, if you hit a target with an attack, gain 1 bonus move. After triggering Relocation, you may move without ending Set Up until the end of your turn.</t>
+  </si>
+  <si>
+    <t>Lucu_Sniper_SabotRound</t>
+  </si>
+  <si>
+    <t>Sabot Round</t>
+  </si>
+  <si>
+    <t>Fire a shot that penetrates obstacles and damages enemies in a line. Ignores cover and 2/4/6 armor on targets. 2 ammo. 4 turn cooldown.</t>
+  </si>
+  <si>
+    <t>Lucu_Sniper_SetUp</t>
+  </si>
+  <si>
+    <t>Set Up</t>
+  </si>
+  <si>
+    <t>You gain Squadsight, but you only gain 1 action point per turn. Your remaining actions may only be used to move this turn. Lasts until you move on following turns.</t>
+  </si>
+  <si>
+    <t>Lucu_Sniper_Sharpshooter</t>
+  </si>
+  <si>
+    <t>Sharpshooter</t>
+  </si>
+  <si>
+    <t>Treat enemies' high cover as low cover for aim purposes.</t>
+  </si>
+  <si>
+    <t>Lucu_Sniper_SniperTraining</t>
+  </si>
+  <si>
+    <t>Sniper Training</t>
+  </si>
+  <si>
+    <t>You may fire sniper rifles for only 1 action point, but with a -15 aim penalty if fired after moving or attacking.</t>
+  </si>
+  <si>
+    <t>Lucu_Sniper_TargetLeading</t>
+  </si>
+  <si>
+    <t>Target Leading</t>
+  </si>
+  <si>
+    <t>You gain +20 aim on reaction fire shots. Enemies suffer -20 dodge against your attacks.</t>
+  </si>
+  <si>
+    <t>Lucu_Sniper_VitalPointTargeting</t>
+  </si>
+  <si>
+    <t>You gain +2/+3/+4 damage with your primary weapon.</t>
+  </si>
+  <si>
+    <t>Lucu_Sniper_ZeroIn</t>
+  </si>
+  <si>
+    <t>You gain +10 aim and +10 crit on your first attack if you did not move last turn. This bonus is lost if you move.</t>
+  </si>
+  <si>
+    <t>BackStabber</t>
+  </si>
+  <si>
+    <t>Backstabber</t>
+  </si>
+  <si>
+    <t>Reduces the cooldown for SilentTakedown by 1 and adds 2 Bonus Damage for Combat Knives.</t>
+  </si>
+  <si>
+    <t>SpecOps Combat Knives</t>
+  </si>
+  <si>
+    <t>Hailstorm</t>
+  </si>
+  <si>
+    <t>Hail Storm</t>
+  </si>
+  <si>
+    <t>Throw three knives at the same target.</t>
+  </si>
+  <si>
+    <t>KnifeJuggler</t>
+  </si>
+  <si>
+    <t>Knife Juggler</t>
+  </si>
+  <si>
+    <t>+ 1 Bonus Damage for the throwing knives and +10 aim when using throwing knives. Also provides one additional charge for the utility throwing knives.</t>
+  </si>
+  <si>
+    <t>ReturnThrow</t>
+  </si>
+  <si>
+    <t>Return Throw</t>
+  </si>
+  <si>
+    <t>When targeted by enemy fire, automatically throw a knife back once per turn.</t>
+  </si>
+  <si>
+    <t>ThrowingKnifeFaceoff</t>
+  </si>
+  <si>
+    <t>House of 1000 Daggers</t>
+  </si>
+  <si>
+    <t>Throw a knife at every visible enemy.</t>
+  </si>
+  <si>
+    <t>ThrowingKnifeQuickdraw</t>
+  </si>
+  <si>
+    <t>Throwing a knive with your first action no longer ends your turn.</t>
+  </si>
+  <si>
+    <t>DangerSense</t>
+  </si>
+  <si>
+    <t>Danger Sense</t>
+  </si>
+  <si>
+    <t>You should be calm outside, but keep your mind alert and prepared. The Samurais keen danger sense tracks movement 20 meters around him. He cannot be surprised be faceless or burrowed chryssalids.</t>
+  </si>
+  <si>
+    <t>LW2 Samurai</t>
+  </si>
+  <si>
+    <t>DragonStrike</t>
+  </si>
+  <si>
+    <t>Dragon Strike</t>
+  </si>
+  <si>
+    <t>Reason will not decide at last; the sword will decide! Unleash a terrible strike upon your enemy, that does aoe damage and can disorient survivers</t>
+  </si>
+  <si>
+    <t>HawkEye</t>
+  </si>
+  <si>
+    <t>Hawkeye</t>
+  </si>
+  <si>
+    <t>According to what one of the elders said, taking an enemy on the battlefield is like a hawk taking a bird. &lt;br/&gt;Even though it enters into the midst of a thousand of them, it gives no attention to any bird than the one it first marked.&lt;br/&gt;Grants +15 critical hit chance and +3 critical damage for melee attacks</t>
+  </si>
+  <si>
+    <t>SamuraiCoupDeGrace</t>
+  </si>
+  <si>
+    <t>SamuraiCutthroat</t>
+  </si>
+  <si>
+    <t>SamuraiFrenzy</t>
+  </si>
+  <si>
+    <t>Shigurui</t>
+  </si>
+  <si>
+    <t>Even if one's head were to be suddenly cut off, he should be able to do one more action with certainty. With martial valor, if one becomes like a revengeful ghost and shows great determination, though his head is cut off, he should not die.&lt;br/&gt;When the Samurai is wounded in battle he enters a death frenzy state and gets 1 additional action point, +80 dodge and +50 crit chance in melee for 2 rounds.</t>
+  </si>
+  <si>
+    <t>SamuraiLightningReflexes_LW</t>
+  </si>
+  <si>
+    <t>The hit chance of reaction fire against this unit is reduced by 90 percent for the first shot, and by 70 percent for additional shots.</t>
+  </si>
+  <si>
+    <t>Shinigami</t>
+  </si>
+  <si>
+    <t>\"Today i become death\" Our scientists are not entirely sure why the Samurai is so much faster than our regular soldiers. They say its a psyonic ability that absorbs the energy of fallen. Each time you kill a living target in melee collect soul. Every two souls grants you one charge of shinigami to boost your AP. &lt;br/&gt;For every 10 souls you collect in total you gain +1 critical chance and for every 20 souls +1 critical damage (melee only, based on overall melee killcount from all battles since shinigami is added)</t>
+  </si>
+  <si>
+    <t>TrainingDiscipline</t>
+  </si>
+  <si>
+    <t>Training Discipline</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;True strength is the flower of Wisdom, but its seed is action.&lt;i/&gt;&lt;br/&gt;The Samurais relentless training provides +3 mobilty and +20 dodge.</t>
+  </si>
+  <si>
+    <t>Unstoppable</t>
+  </si>
+  <si>
+    <t>In the words of the ancients, one should make his decision within the space of seven breaths.&lt;br/&gt;It is a matter of being determined and having the spirit to break through to the other side.&lt;br/&gt;Melee attacks never graze</t>
+  </si>
+  <si>
+    <t>WayOfTheSamurai</t>
+  </si>
+  <si>
+    <t>Way of the Samurai</t>
+  </si>
+  <si>
+    <t>The Way of the Samurai is found in death. Meditation on inevitable death should be performed daily.&lt;br/&gt;The intensive swordtraining adds +3 damage and +10 hit chance with melee weapons.</t>
+  </si>
+  <si>
+    <t>WhirlwindStrike</t>
+  </si>
+  <si>
+    <t>Whirlwind Strike</t>
+  </si>
+  <si>
+    <t>The Way of the Samurai is one of immediacy, and it is best to dash in headlong.&lt;br/&gt;Perfom two slashes at the target. Each has an aim penalty of -15.&lt;br/&gt;No cooldown.</t>
+  </si>
+  <si>
+    <t>Yamabushi</t>
+  </si>
+  <si>
+    <t>Yamabushi Heritage</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;The Shugendo disciples search for spiritual, mystical, or supernatural powers gained through asceticism&lt;i/&gt;You are strong as the montain and gain +1 armor, +15 defense and can regenerate 2 HP per round, max to 6 HP.</t>
   </si>
 </sst>
 </file>
@@ -3799,7 +4612,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G392"/>
+  <dimension ref="A1:G487"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
       <selection activeCell="F76" sqref="F76"/>
@@ -10696,6 +11509,1621 @@
       </c>
       <c r="E392" s="0" t="s">
         <v>259</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" s="0" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B393" s="0" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C393" s="0" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D393" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E393" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B394" s="0" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C394" s="0" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D394" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E394" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" s="0" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B395" s="0" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C395" s="0" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D395" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E395" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" s="0" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B396" s="0" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C396" s="0" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D396" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E396" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" s="0" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B397" s="0" t="s">
+        <v>824</v>
+      </c>
+      <c r="C397" s="0" t="s">
+        <v>1160</v>
+      </c>
+      <c r="D397" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E397" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" s="0" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B398" s="0" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C398" s="0" t="s">
+        <v>1163</v>
+      </c>
+      <c r="D398" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E398" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" s="0" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B399" s="0" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C399" s="0" t="s">
+        <v>1166</v>
+      </c>
+      <c r="D399" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E399" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" s="0" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B400" s="0" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C400" s="0" t="s">
+        <v>1169</v>
+      </c>
+      <c r="D400" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E400" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" s="0" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B401" s="0" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C401" s="0" t="s">
+        <v>1172</v>
+      </c>
+      <c r="D401" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E401" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" s="0" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B402" s="0" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C402" s="0" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D402" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E402" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" s="0" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B403" s="0" t="s">
+        <v>1177</v>
+      </c>
+      <c r="C403" s="0" t="s">
+        <v>1178</v>
+      </c>
+      <c r="D403" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E403" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" s="0" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B404" s="0" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C404" s="0" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D404" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E404" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" s="0" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B405" s="0" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C405" s="0" t="s">
+        <v>1184</v>
+      </c>
+      <c r="D405" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E405" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" s="0" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B406" s="0" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C406" s="0" t="s">
+        <v>1187</v>
+      </c>
+      <c r="D406" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E406" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" s="0" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B407" s="0" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C407" s="0" t="s">
+        <v>1190</v>
+      </c>
+      <c r="D407" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E407" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" s="0" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B408" s="0" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C408" s="0" t="s">
+        <v>1193</v>
+      </c>
+      <c r="D408" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E408" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" s="0" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B409" s="0" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C409" s="0" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D409" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E409" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" s="0" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B410" s="0" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C410" s="0" t="s">
+        <v>1199</v>
+      </c>
+      <c r="D410" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E410" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" s="0" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B411" s="0" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C411" s="0" t="s">
+        <v>1202</v>
+      </c>
+      <c r="D411" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E411" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" s="0" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B412" s="0" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C412" s="0" t="s">
+        <v>1205</v>
+      </c>
+      <c r="D412" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E412" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" s="0" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B413" s="0" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C413" s="0" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D413" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E413" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" s="0" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B414" s="0" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C414" s="0" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D414" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E414" s="0" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" s="0" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B415" s="0" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C415" s="0" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D415" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E415" s="0" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" s="0" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B416" s="0" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C416" s="0" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D416" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E416" s="0" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" s="0" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B417" s="0" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C417" s="0" t="s">
+        <v>1221</v>
+      </c>
+      <c r="D417" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E417" s="0" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" s="0" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B418" s="0" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C418" s="0" t="s">
+        <v>1224</v>
+      </c>
+      <c r="D418" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E418" s="0" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" s="0" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B419" s="0" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C419" s="0" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D419" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E419" s="0" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" s="0" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B420" s="0" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C420" s="0" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D420" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E420" s="0" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" s="0" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B421" s="0" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C421" s="0" t="s">
+        <v>1233</v>
+      </c>
+      <c r="D421" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E421" s="0" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" s="0" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B422" s="0" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C422" s="0" t="s">
+        <v>1236</v>
+      </c>
+      <c r="D422" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E422" s="0" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" s="0" t="s">
+        <v>1237</v>
+      </c>
+      <c r="B423" s="0" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C423" s="0" t="s">
+        <v>1239</v>
+      </c>
+      <c r="D423" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E423" s="0" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" s="0" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B424" s="0" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C424" s="0" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D424" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E424" s="0" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" s="0" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B425" s="0" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C425" s="0" t="s">
+        <v>1245</v>
+      </c>
+      <c r="D425" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E425" s="0" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" s="0" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B426" s="0" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C426" s="0" t="s">
+        <v>1248</v>
+      </c>
+      <c r="D426" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E426" s="0" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" s="0" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B427" s="0" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C427" s="0" t="s">
+        <v>1251</v>
+      </c>
+      <c r="D427" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E427" s="0" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" s="0" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B428" s="0" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C428" s="0" t="s">
+        <v>1254</v>
+      </c>
+      <c r="D428" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E428" s="0" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" s="0" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B429" s="0" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C429" s="0" t="s">
+        <v>1257</v>
+      </c>
+      <c r="D429" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E429" s="0" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" s="0" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B430" s="0" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C430" s="0" t="s">
+        <v>1260</v>
+      </c>
+      <c r="D430" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E430" s="0" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" s="0" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B431" s="0" t="s">
+        <v>991</v>
+      </c>
+      <c r="C431" s="0" t="s">
+        <v>1263</v>
+      </c>
+      <c r="D431" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E431" s="0" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" s="0" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B432" s="0" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C432" s="0" t="s">
+        <v>1266</v>
+      </c>
+      <c r="D432" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E432" s="0" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" s="0" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B433" s="0" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C433" s="0" t="s">
+        <v>1269</v>
+      </c>
+      <c r="D433" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E433" s="0" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B434" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C434" s="0" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D434" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E434" s="0" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" s="0" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B435" s="0" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C435" s="0" t="s">
+        <v>1274</v>
+      </c>
+      <c r="D435" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E435" s="0" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" s="0" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B436" s="0" t="s">
+        <v>795</v>
+      </c>
+      <c r="C436" s="0" t="s">
+        <v>1276</v>
+      </c>
+      <c r="D436" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E436" s="0" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" s="0" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B437" s="0" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C437" s="0" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D437" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E437" s="0" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" s="0" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B438" s="0" t="s">
+        <v>730</v>
+      </c>
+      <c r="C438" s="0" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D438" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E438" s="0" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" s="0" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B439" s="0" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C439" s="0" t="s">
+        <v>1283</v>
+      </c>
+      <c r="D439" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E439" s="0" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" s="0" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B440" s="0" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C440" s="0" t="s">
+        <v>1286</v>
+      </c>
+      <c r="D440" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E440" s="0" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" s="0" t="s">
+        <v>1287</v>
+      </c>
+      <c r="B441" s="0" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C441" s="0" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D441" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E441" s="0" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" s="0" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B442" s="0" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C442" s="0" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D442" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E442" s="0" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" s="0" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B443" s="0" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C443" s="0" t="s">
+        <v>1295</v>
+      </c>
+      <c r="D443" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E443" s="0" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" s="0" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B444" s="0" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C444" s="0" t="s">
+        <v>1298</v>
+      </c>
+      <c r="D444" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E444" s="0" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" s="0" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B445" s="0" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C445" s="0" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D445" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E445" s="0" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" s="0" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B446" s="0" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C446" s="0" t="s">
+        <v>1304</v>
+      </c>
+      <c r="D446" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E446" s="0" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" s="0" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B447" s="0" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C447" s="0" t="s">
+        <v>1307</v>
+      </c>
+      <c r="D447" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E447" s="0" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" s="0" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B448" s="0" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C448" s="0" t="s">
+        <v>1310</v>
+      </c>
+      <c r="D448" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E448" s="0" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" s="0" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B449" s="0" t="s">
+        <v>864</v>
+      </c>
+      <c r="C449" s="0" t="s">
+        <v>865</v>
+      </c>
+      <c r="D449" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E449" s="0" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" s="0" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B450" s="0" t="s">
+        <v>1313</v>
+      </c>
+      <c r="C450" s="0" t="s">
+        <v>1314</v>
+      </c>
+      <c r="D450" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E450" s="0" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" s="0" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B451" s="0" t="s">
+        <v>1316</v>
+      </c>
+      <c r="C451" s="0" t="s">
+        <v>1317</v>
+      </c>
+      <c r="D451" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E451" s="0" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" s="0" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B452" s="0" t="s">
+        <v>1319</v>
+      </c>
+      <c r="C452" s="0" t="s">
+        <v>1320</v>
+      </c>
+      <c r="D452" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E452" s="0" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" s="0" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B453" s="0" t="s">
+        <v>1322</v>
+      </c>
+      <c r="C453" s="0" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D453" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E453" s="0" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" s="0" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B454" s="0" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C454" s="0" t="s">
+        <v>1326</v>
+      </c>
+      <c r="D454" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E454" s="0" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" s="0" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B455" s="0" t="s">
+        <v>1329</v>
+      </c>
+      <c r="C455" s="0" t="s">
+        <v>1330</v>
+      </c>
+      <c r="D455" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E455" s="0" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" s="0" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B456" s="0" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C456" s="0" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D456" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E456" s="0" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" s="0" t="s">
+        <v>1334</v>
+      </c>
+      <c r="B457" s="0" t="s">
+        <v>1335</v>
+      </c>
+      <c r="C457" s="0" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D457" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E457" s="0" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" s="0" t="s">
+        <v>1337</v>
+      </c>
+      <c r="B458" s="0" t="s">
+        <v>1338</v>
+      </c>
+      <c r="C458" s="0" t="s">
+        <v>1339</v>
+      </c>
+      <c r="D458" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E458" s="0" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" s="0" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B459" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="C459" s="0" t="s">
+        <v>1341</v>
+      </c>
+      <c r="D459" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E459" s="0" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" s="0" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B460" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="C460" s="0" t="s">
+        <v>1343</v>
+      </c>
+      <c r="D460" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E460" s="0" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" s="0" t="s">
+        <v>1344</v>
+      </c>
+      <c r="B461" s="0" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C461" s="0" t="s">
+        <v>1346</v>
+      </c>
+      <c r="D461" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E461" s="0" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" s="0" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B462" s="0" t="s">
+        <v>1348</v>
+      </c>
+      <c r="C462" s="0" t="s">
+        <v>1349</v>
+      </c>
+      <c r="D462" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E462" s="0" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" s="0" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B463" s="0" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C463" s="0" t="s">
+        <v>1352</v>
+      </c>
+      <c r="D463" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E463" s="0" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" s="0" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B464" s="0" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C464" s="0" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D464" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E464" s="0" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" s="0" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B465" s="0" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C465" s="0" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D465" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E465" s="0" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" s="0" t="s">
+        <v>1359</v>
+      </c>
+      <c r="B466" s="0" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C466" s="0" t="s">
+        <v>1361</v>
+      </c>
+      <c r="D466" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E466" s="0" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" s="0" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B467" s="0" t="s">
+        <v>599</v>
+      </c>
+      <c r="C467" s="0" t="s">
+        <v>1363</v>
+      </c>
+      <c r="D467" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E467" s="0" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" s="0" t="s">
+        <v>1364</v>
+      </c>
+      <c r="B468" s="0" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C468" s="0" t="s">
+        <v>1365</v>
+      </c>
+      <c r="D468" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E468" s="0" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" s="0" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B469" s="0" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C469" s="0" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D469" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E469" s="0" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" s="0" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B470" s="0" t="s">
+        <v>1371</v>
+      </c>
+      <c r="C470" s="0" t="s">
+        <v>1372</v>
+      </c>
+      <c r="D470" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E470" s="0" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" s="0" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B471" s="0" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C471" s="0" t="s">
+        <v>1375</v>
+      </c>
+      <c r="D471" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E471" s="0" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" s="0" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B472" s="0" t="s">
+        <v>1377</v>
+      </c>
+      <c r="C472" s="0" t="s">
+        <v>1378</v>
+      </c>
+      <c r="D472" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E472" s="0" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" s="0" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B473" s="0" t="s">
+        <v>1380</v>
+      </c>
+      <c r="C473" s="0" t="s">
+        <v>1381</v>
+      </c>
+      <c r="D473" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E473" s="0" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" s="0" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B474" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C474" s="0" t="s">
+        <v>1383</v>
+      </c>
+      <c r="D474" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E474" s="0" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" s="0" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B475" s="0" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C475" s="0" t="s">
+        <v>1386</v>
+      </c>
+      <c r="D475" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E475" s="0" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" s="0" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B476" s="0" t="s">
+        <v>1389</v>
+      </c>
+      <c r="C476" s="0" t="s">
+        <v>1390</v>
+      </c>
+      <c r="D476" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E476" s="0" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" s="0" t="s">
+        <v>1391</v>
+      </c>
+      <c r="B477" s="0" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C477" s="0" t="s">
+        <v>1393</v>
+      </c>
+      <c r="D477" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E477" s="0" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" s="0" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B478" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="C478" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="D478" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E478" s="0" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" s="0" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B479" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="C479" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="D479" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E479" s="0" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" s="0" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B480" s="0" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C480" s="0" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D480" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E480" s="0" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" s="0" t="s">
+        <v>1399</v>
+      </c>
+      <c r="B481" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C481" s="0" t="s">
+        <v>1400</v>
+      </c>
+      <c r="D481" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E481" s="0" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" s="0" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B482" s="0" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C482" s="0" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D482" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E482" s="0" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" s="0" t="s">
+        <v>1403</v>
+      </c>
+      <c r="B483" s="0" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C483" s="0" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D483" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E483" s="0" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" s="0" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B484" s="0" t="s">
+        <v>1406</v>
+      </c>
+      <c r="C484" s="0" t="s">
+        <v>1407</v>
+      </c>
+      <c r="D484" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E484" s="0" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" s="0" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B485" s="0" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C485" s="0" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D485" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E485" s="0" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" s="0" t="s">
+        <v>1411</v>
+      </c>
+      <c r="B486" s="0" t="s">
+        <v>1412</v>
+      </c>
+      <c r="C486" s="0" t="s">
+        <v>1413</v>
+      </c>
+      <c r="D486" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E486" s="0" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" s="0" t="s">
+        <v>1414</v>
+      </c>
+      <c r="B487" s="0" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C487" s="0" t="s">
+        <v>1416</v>
+      </c>
+      <c r="D487" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E487" s="0" t="s">
+        <v>1387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Imported a bunch of abilities.
</commit_message>
<xml_diff>
--- a/Xcom2ClassManager/XComAbilityList.xlsx
+++ b/Xcom2ClassManager/XComAbilityList.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="1417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="1597">
   <si>
     <t>Name</t>
   </si>
@@ -4270,6 +4270,546 @@
   </si>
   <si>
     <t>&lt;i&gt;The Shugendo disciples search for spiritual, mystical, or supernatural powers gained through asceticism&lt;i/&gt;You are strong as the montain and gain +1 armor, +15 defense and can regenerate 2 HP per round, max to 6 HP.</t>
+  </si>
+  <si>
+    <t>JuggAdaptingArmor</t>
+  </si>
+  <si>
+    <t>Adaptive Armor</t>
+  </si>
+  <si>
+    <t>Takes 2 less damage from all attacks for 2 turns after taking damage.</t>
+  </si>
+  <si>
+    <t>Juggernaut</t>
+  </si>
+  <si>
+    <t>JuggDamageControl</t>
+  </si>
+  <si>
+    <t>Grants 2 additional armor.</t>
+  </si>
+  <si>
+    <t>JuggDimensionalShift</t>
+  </si>
+  <si>
+    <t>Shields Overload</t>
+  </si>
+  <si>
+    <t>Expending all the shield energy within a short time, provides immunity to damage this turn, while in this state, the unit also fools the enemies as an easy target.</t>
+  </si>
+  <si>
+    <t>JuggDisorientationField</t>
+  </si>
+  <si>
+    <t>Disorientation Field</t>
+  </si>
+  <si>
+    <t>Disorients nearby enemies at the end of each turn.</t>
+  </si>
+  <si>
+    <t>JuggDistortionField</t>
+  </si>
+  <si>
+    <t>Group Protective Field</t>
+  </si>
+  <si>
+    <t>Produces a large protective field that reduces accuracy by 15% against any nearby squadmates.</t>
+  </si>
+  <si>
+    <t>JuggEnergyShield</t>
+  </si>
+  <si>
+    <t>Energy Shield</t>
+  </si>
+  <si>
+    <t>Generates a 5hp shield for nearby allies throughout the enemy turn.</t>
+  </si>
+  <si>
+    <t>JuggHeavyArmor</t>
+  </si>
+  <si>
+    <t>Heavy Armor</t>
+  </si>
+  <si>
+    <t>The armor absorbs damage taken, protecting the wearer from injury.</t>
+  </si>
+  <si>
+    <t>JuggHighCover</t>
+  </si>
+  <si>
+    <t>One for all</t>
+  </si>
+  <si>
+    <t>Become a heavy cover until an offensive action is taken.</t>
+  </si>
+  <si>
+    <t>JuggProtect</t>
+  </si>
+  <si>
+    <t>Defender's Will</t>
+  </si>
+  <si>
+    <t>Goes into a defensive stance, attacking any enemy who attacks in range until the soldier runs out of ammunition</t>
+  </si>
+  <si>
+    <t>JuggRegen</t>
+  </si>
+  <si>
+    <t>Feel No Pain</t>
+  </si>
+  <si>
+    <t>HP damage taken instantly gets regenerated as shields.</t>
+  </si>
+  <si>
+    <t>JuggResilient</t>
+  </si>
+  <si>
+    <t>Resilient</t>
+  </si>
+  <si>
+    <t>Become 15% harder to land a critical shot, and an additional 30% if flanked.</t>
+  </si>
+  <si>
+    <t>JuggShockAbsorbantArmor</t>
+  </si>
+  <si>
+    <t>Reduce damage taken by 66% from nearby sources.</t>
+  </si>
+  <si>
+    <t>JuggThreatPrediction</t>
+  </si>
+  <si>
+    <t>Shaped Armor</t>
+  </si>
+  <si>
+    <t>Increases dodge by 75% for a turn</t>
+  </si>
+  <si>
+    <t>JackArmorPadding</t>
+  </si>
+  <si>
+    <t>Armor Padding</t>
+  </si>
+  <si>
+    <t>Gain +3 HP and receive an additional +10 Defense bonus. Less susceptible to stuns.</t>
+  </si>
+  <si>
+    <t>Trooper</t>
+  </si>
+  <si>
+    <t>JackArtOfWar</t>
+  </si>
+  <si>
+    <t>Art of War</t>
+  </si>
+  <si>
+    <t>Deal +2 bonus damage to flanked enemies, with a +15% critical chance bonus.</t>
+  </si>
+  <si>
+    <t>JackDeathSentence</t>
+  </si>
+  <si>
+    <t>Death Sentence</t>
+  </si>
+  <si>
+    <t>Brace yourself. Fire a reaction shot for every enemy action within a radius. -20 Defense penalty. 5-turn cooldown.</t>
+  </si>
+  <si>
+    <t>JackLastStand</t>
+  </si>
+  <si>
+    <t>Survivor</t>
+  </si>
+  <si>
+    <t>Falling in battle heals the Trooper for 5HP and grants a +20 bonus to Will and Defense for the remaining battle. Once per battle.</t>
+  </si>
+  <si>
+    <t>JackLethalShot</t>
+  </si>
+  <si>
+    <t>Lethal Shot</t>
+  </si>
+  <si>
+    <t>Deal +1 bonus damage on attacks with a +5% Critical chance. Your attacks always graze enemies.</t>
+  </si>
+  <si>
+    <t>JackMarkTarget</t>
+  </si>
+  <si>
+    <t>Mark Target</t>
+  </si>
+  <si>
+    <t>Mark a target for 2 turns. All allies gain +15 Aim bonus when attacking the target.</t>
+  </si>
+  <si>
+    <t>JackPiercingBarrage</t>
+  </si>
+  <si>
+    <t>Piercing Barrage</t>
+  </si>
+  <si>
+    <t>Unleash a barrage of piercing rounds, damaging cover and enemies in a straight line. Penalty to aim and damage. Costs 2 ammo. 4-turn cooldown.</t>
+  </si>
+  <si>
+    <t>JackScatter</t>
+  </si>
+  <si>
+    <t>Spread Out</t>
+  </si>
+  <si>
+    <t>Nearby allies gain a 20% Dodge bonus for the next 2 turns, and a temporary boost to mobility. 4-turn cooldown.</t>
+  </si>
+  <si>
+    <t>JackSurvivalInstinct</t>
+  </si>
+  <si>
+    <t>Getting hit by an attack grants a +25 Defense and +5 Aim for one turn.</t>
+  </si>
+  <si>
+    <t>JackTactics</t>
+  </si>
+  <si>
+    <t>Aggressive Tactics</t>
+  </si>
+  <si>
+    <t>Increases target's Aim by +5, Damage by +3, and a provides a great boost to mobility for one turn, with a -10 Defense penalty. 4 turn cooldown.</t>
+  </si>
+  <si>
+    <t>JackTrueShot</t>
+  </si>
+  <si>
+    <t>Lucky Shot</t>
+  </si>
+  <si>
+    <t>Unleash a focused shot from your pistol that ignores enemy armor. Guaranteed to hit. 3-turn cooldown.</t>
+  </si>
+  <si>
+    <t>KeenEye</t>
+  </si>
+  <si>
+    <t>Gain a +5 Defense bonus and a 5% bonus to critically hit enemies.</t>
+  </si>
+  <si>
+    <t>BlastShot</t>
+  </si>
+  <si>
+    <t>Share Blast</t>
+  </si>
+  <si>
+    <t>Fire a blast of energy in a narrow, long path in front of you. Can recieve +2 from HDD.</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>HDD</t>
+  </si>
+  <si>
+    <t>Sacrifice 15 Defense for +2 damage, +20 aim and +25 crit. Can chain into other abilities! This health cannot be recovered until your next turn</t>
+  </si>
+  <si>
+    <t>NepBull</t>
+  </si>
+  <si>
+    <t>Nep Bull</t>
+  </si>
+  <si>
+    <t>Self-use drink that restores up to 4 health to the user. 2 Uses per battle.</t>
+  </si>
+  <si>
+    <t>NextGen</t>
+  </si>
+  <si>
+    <t>Next Gen</t>
+  </si>
+  <si>
+    <t>One of the CPU's Gamechangers. Strike all foes in range with a pistol. Inflicts stun on FIRST TARGET. Can chain from HDD.</t>
+  </si>
+  <si>
+    <t>PartBreak</t>
+  </si>
+  <si>
+    <t>Part Break</t>
+  </si>
+  <si>
+    <t>Attack that focuses on breaking foe's armor, shredding up to 6 points. 3 Uses.</t>
+  </si>
+  <si>
+    <t>Patience</t>
+  </si>
+  <si>
+    <t>Wait for an opening from the enemy. This attack deals 2 bonus damage and is guaranteed to hit. Can chain from HDD for +4 Damage.</t>
+  </si>
+  <si>
+    <t>Prioritize</t>
+  </si>
+  <si>
+    <t>Mark a taget, giveing everyone (Including yourself) +10 Aim on it.</t>
+  </si>
+  <si>
+    <t>Sentient</t>
+  </si>
+  <si>
+    <t>Ends turn with +10 Armor until the start of the next turn. Helps avoid death in tight spots.</t>
+  </si>
+  <si>
+    <t>Smite</t>
+  </si>
+  <si>
+    <t>Pistol attack that causes the enemy to panic. Deals no damage however (Cannot gain +2 from HDD)</t>
+  </si>
+  <si>
+    <t>Swiftness</t>
+  </si>
+  <si>
+    <t>Increases Mobility stat by 2 points.</t>
+  </si>
+  <si>
+    <t>Teleport</t>
+  </si>
+  <si>
+    <t>Warp</t>
+  </si>
+  <si>
+    <t>One of the CPU's Gamechangers. Allows the user to warp to another location.</t>
+  </si>
+  <si>
+    <t>NecroCombustion</t>
+  </si>
+  <si>
+    <t>Combustion</t>
+  </si>
+  <si>
+    <t>Cause a creature's blood to boil. Does 2-4 guaranteed psi damage and sets them on fire.</t>
+  </si>
+  <si>
+    <t>Necromancer</t>
+  </si>
+  <si>
+    <t>NecroDeathTouch</t>
+  </si>
+  <si>
+    <t>Death Touch</t>
+  </si>
+  <si>
+    <t>The Necromancer has gained a superhuman understanding of life and death. Touch a living creature to grab its soul and pull it out of its body. It dies instantly. It can be used once per battle, from melee range only.</t>
+  </si>
+  <si>
+    <t>NecroDrainLife</t>
+  </si>
+  <si>
+    <t>Drain Life</t>
+  </si>
+  <si>
+    <t>Shoots a target enemy and transfers half of the damage done back to the Necromancer as health.</t>
+  </si>
+  <si>
+    <t>NecroEldritchStorm</t>
+  </si>
+  <si>
+    <t>Eldritch Storm</t>
+  </si>
+  <si>
+    <t>The necromancer has become an avatar of death. Focus all your power into one spell that will Set on Fire, Poison,and cause Acid Burn to all enemies in a large radius. Does no direct damage.</t>
+  </si>
+  <si>
+    <t>NecroFireballAbility</t>
+  </si>
+  <si>
+    <t>Fireball</t>
+  </si>
+  <si>
+    <t>Launch a Fireball, dealing explosive damage to everyone in the blast radius and setting everything on fire.</t>
+  </si>
+  <si>
+    <t>NecroHallucination</t>
+  </si>
+  <si>
+    <t>Hallucinations curse</t>
+  </si>
+  <si>
+    <t>The necromancer curses a creature, causing them to see their own team as enemies, and then overloads its mind with impending doom. Surrounded from all sides, they are guaranteed to panic, unless they have full immunity to panic. There is a good chance they will shoot their own team.</t>
+  </si>
+  <si>
+    <t>NecroLightning</t>
+  </si>
+  <si>
+    <t>Lightning</t>
+  </si>
+  <si>
+    <t>Shoots a lightning bolt at a target location. Damages everyone caught in the radius, stuns organic units and causes robotic ones to reboot. Costs 2 action points.</t>
+  </si>
+  <si>
+    <t>NecroMassRaiseDead</t>
+  </si>
+  <si>
+    <t>Army of the dead</t>
+  </si>
+  <si>
+    <t>Raises all dead humans in a large radius as zombies.</t>
+  </si>
+  <si>
+    <t>NecroPoison</t>
+  </si>
+  <si>
+    <t>Poison</t>
+  </si>
+  <si>
+    <t>Poison any living, organic creature. Does 1 damage per turn, -30 to aim and -4 to move. The spell doesn't end your turn and has no cooldown.</t>
+  </si>
+  <si>
+    <t>NecroRaiseDead</t>
+  </si>
+  <si>
+    <t>Raise Zombie</t>
+  </si>
+  <si>
+    <t>Raise a dead human or Advent as a zombie with 8 HP.</t>
+  </si>
+  <si>
+    <t>NecroRestoration</t>
+  </si>
+  <si>
+    <t>Regenerate 1 HP per turn, for 3 turns, to any ally. \n Shamans are said to treat ailments/illness by mending the soul. Alleviating traumas affecting the soul/spirit restores the physical body of the individual to balance and wholeness.</t>
+  </si>
+  <si>
+    <t>NecroSoulSpear</t>
+  </si>
+  <si>
+    <t>Soul Spear</t>
+  </si>
+  <si>
+    <t>Sorcery that fires souls shaped into a spear. Pierces enemies, causing heavy damage. This spell was said to have been devised by a master sorcerer, but his name is long forgotten.</t>
+  </si>
+  <si>
+    <t>NecroSpiritArmorAbility</t>
+  </si>
+  <si>
+    <t>Bone Armor</t>
+  </si>
+  <si>
+    <t>Adds 3 armor to a friendly target. This bonus lasts until the end of the mission and can be stacked. 4 turns cool down.</t>
+  </si>
+  <si>
+    <t>NecroStrenghtenUndead</t>
+  </si>
+  <si>
+    <t>Undead Link</t>
+  </si>
+  <si>
+    <t>Enhance the link between the Necromancer and one of his zombies, significantly increasing all of its life stats.</t>
+  </si>
+  <si>
+    <t>AbsorptionField</t>
+  </si>
+  <si>
+    <t>Channeling Field</t>
+  </si>
+  <si>
+    <t>Every time you are targeted, part of the energy is channeled to your &lt;Ability:WeaponName&gt;. This energy is unleashed with your next Standard Shot.</t>
+  </si>
+  <si>
+    <t>Shen's Last Gift</t>
+  </si>
+  <si>
+    <t>AdaptiveAim</t>
+  </si>
+  <si>
+    <t>Adaptive Aim</t>
+  </si>
+  <si>
+    <t>When Overdrive is active, Standard Shots do not incur recoil penalties.</t>
+  </si>
+  <si>
+    <t>Arsenal</t>
+  </si>
+  <si>
+    <t>The BIT can equip and fire heavy weapons.</t>
+  </si>
+  <si>
+    <t>Bombard</t>
+  </si>
+  <si>
+    <t>Launch the BIT to any visible location where it releases a powerful explosive blast. Advanced BITs do more damage.</t>
+  </si>
+  <si>
+    <t>Bulwark</t>
+  </si>
+  <si>
+    <t>Gain a bonus point of Armor, and always provide high cover to all adjacent squadmates.</t>
+  </si>
+  <si>
+    <t>CapacitorDischarge_Shen</t>
+  </si>
+  <si>
+    <t>CombatProtocol_Shen</t>
+  </si>
+  <si>
+    <t>HunterProtocol</t>
+  </si>
+  <si>
+    <t>Hunter Protocol</t>
+  </si>
+  <si>
+    <t>When an enemy is revealed, there is a &lt;Ability:HunterProtocol_Chance/&gt;% chance to take a free Overwatch shot.</t>
+  </si>
+  <si>
+    <t>Intimidate</t>
+  </si>
+  <si>
+    <t>When targeted by an attack, the enemy has a chance to panic.</t>
+  </si>
+  <si>
+    <t>MedicalProtocol_Shen</t>
+  </si>
+  <si>
+    <t>The GREMLIN can perform healing actions remotely: GREMLIN Heal and GREMLIN Stabilize. The GREMLIN has four charges. If a medikit is equipped, the GREMLIN will gain an additional charge.</t>
+  </si>
+  <si>
+    <t>Nova</t>
+  </si>
+  <si>
+    <t>Release a blast of energy, damaging all nearby enemies. This attack has no cost or cooldown, but consecutive Novas will damage the SPARK.</t>
+  </si>
+  <si>
+    <t>Overdrive</t>
+  </si>
+  <si>
+    <t>Take three actions this turn, and no action is turn-ending. Multiple Standard Shots incur a small recoil penalty.</t>
+  </si>
+  <si>
+    <t>Rainmaker</t>
+  </si>
+  <si>
+    <t>Equipped heavy weapons deal +&lt;Ability:Rainmaker_BonusDamage/&gt; damage and have increased area of effect.</t>
+  </si>
+  <si>
+    <t>Repair</t>
+  </si>
+  <si>
+    <t>Send the BIT to a damaged robotic ally and repair it. Advanced BITs can repair slightly more.</t>
+  </si>
+  <si>
+    <t>Sacrifice</t>
+  </si>
+  <si>
+    <t>Generate a protective field which redirects any attacks against allies inside it towards you. Gain bonus defense and armor while active.</t>
+  </si>
+  <si>
+    <t>Strike</t>
+  </si>
+  <si>
+    <t>Attack any enemy within movement range with a powerful melee attack.</t>
+  </si>
+  <si>
+    <t>WreckingBall</t>
+  </si>
+  <si>
+    <t>Wrecking Ball</t>
+  </si>
+  <si>
+    <t>While Overdrive is active, break through walls and cover when moving.</t>
   </si>
 </sst>
 </file>
@@ -4612,7 +5152,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G487"/>
+  <dimension ref="A1:G554"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
       <selection activeCell="F76" sqref="F76"/>
@@ -13124,6 +13664,1145 @@
       </c>
       <c r="E487" s="0" t="s">
         <v>1387</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" s="0" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B488" s="0" t="s">
+        <v>1418</v>
+      </c>
+      <c r="C488" s="0" t="s">
+        <v>1419</v>
+      </c>
+      <c r="D488" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E488" s="0" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" s="0" t="s">
+        <v>1421</v>
+      </c>
+      <c r="B489" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="C489" s="0" t="s">
+        <v>1422</v>
+      </c>
+      <c r="D489" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E489" s="0" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" s="0" t="s">
+        <v>1423</v>
+      </c>
+      <c r="B490" s="0" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C490" s="0" t="s">
+        <v>1425</v>
+      </c>
+      <c r="D490" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E490" s="0" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" s="0" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B491" s="0" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C491" s="0" t="s">
+        <v>1428</v>
+      </c>
+      <c r="D491" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E491" s="0" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" s="0" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B492" s="0" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C492" s="0" t="s">
+        <v>1431</v>
+      </c>
+      <c r="D492" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E492" s="0" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" s="0" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B493" s="0" t="s">
+        <v>1433</v>
+      </c>
+      <c r="C493" s="0" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D493" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E493" s="0" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" s="0" t="s">
+        <v>1435</v>
+      </c>
+      <c r="B494" s="0" t="s">
+        <v>1436</v>
+      </c>
+      <c r="C494" s="0" t="s">
+        <v>1437</v>
+      </c>
+      <c r="D494" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E494" s="0" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" s="0" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B495" s="0" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C495" s="0" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D495" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E495" s="0" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" s="0" t="s">
+        <v>1441</v>
+      </c>
+      <c r="B496" s="0" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C496" s="0" t="s">
+        <v>1443</v>
+      </c>
+      <c r="D496" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E496" s="0" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" s="0" t="s">
+        <v>1444</v>
+      </c>
+      <c r="B497" s="0" t="s">
+        <v>1445</v>
+      </c>
+      <c r="C497" s="0" t="s">
+        <v>1446</v>
+      </c>
+      <c r="D497" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E497" s="0" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" s="0" t="s">
+        <v>1447</v>
+      </c>
+      <c r="B498" s="0" t="s">
+        <v>1448</v>
+      </c>
+      <c r="C498" s="0" t="s">
+        <v>1449</v>
+      </c>
+      <c r="D498" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E498" s="0" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" s="0" t="s">
+        <v>1450</v>
+      </c>
+      <c r="B499" s="0" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C499" s="0" t="s">
+        <v>1451</v>
+      </c>
+      <c r="D499" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E499" s="0" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" s="0" t="s">
+        <v>1452</v>
+      </c>
+      <c r="B500" s="0" t="s">
+        <v>1453</v>
+      </c>
+      <c r="C500" s="0" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D500" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E500" s="0" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" s="0" t="s">
+        <v>1455</v>
+      </c>
+      <c r="B501" s="0" t="s">
+        <v>1456</v>
+      </c>
+      <c r="C501" s="0" t="s">
+        <v>1457</v>
+      </c>
+      <c r="D501" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E501" s="0" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" s="0" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B502" s="0" t="s">
+        <v>1460</v>
+      </c>
+      <c r="C502" s="0" t="s">
+        <v>1461</v>
+      </c>
+      <c r="D502" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E502" s="0" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" s="0" t="s">
+        <v>1462</v>
+      </c>
+      <c r="B503" s="0" t="s">
+        <v>1463</v>
+      </c>
+      <c r="C503" s="0" t="s">
+        <v>1464</v>
+      </c>
+      <c r="D503" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E503" s="0" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" s="0" t="s">
+        <v>1465</v>
+      </c>
+      <c r="B504" s="0" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C504" s="0" t="s">
+        <v>1467</v>
+      </c>
+      <c r="D504" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E504" s="0" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" s="0" t="s">
+        <v>1468</v>
+      </c>
+      <c r="B505" s="0" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C505" s="0" t="s">
+        <v>1470</v>
+      </c>
+      <c r="D505" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E505" s="0" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" s="0" t="s">
+        <v>1471</v>
+      </c>
+      <c r="B506" s="0" t="s">
+        <v>1472</v>
+      </c>
+      <c r="C506" s="0" t="s">
+        <v>1473</v>
+      </c>
+      <c r="D506" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E506" s="0" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" s="0" t="s">
+        <v>1474</v>
+      </c>
+      <c r="B507" s="0" t="s">
+        <v>1475</v>
+      </c>
+      <c r="C507" s="0" t="s">
+        <v>1476</v>
+      </c>
+      <c r="D507" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E507" s="0" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" s="0" t="s">
+        <v>1477</v>
+      </c>
+      <c r="B508" s="0" t="s">
+        <v>1478</v>
+      </c>
+      <c r="C508" s="0" t="s">
+        <v>1479</v>
+      </c>
+      <c r="D508" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E508" s="0" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" s="0" t="s">
+        <v>1480</v>
+      </c>
+      <c r="B509" s="0" t="s">
+        <v>898</v>
+      </c>
+      <c r="C509" s="0" t="s">
+        <v>1481</v>
+      </c>
+      <c r="D509" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E509" s="0" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" s="0" t="s">
+        <v>1482</v>
+      </c>
+      <c r="B510" s="0" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C510" s="0" t="s">
+        <v>1484</v>
+      </c>
+      <c r="D510" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E510" s="0" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" s="0" t="s">
+        <v>1485</v>
+      </c>
+      <c r="B511" s="0" t="s">
+        <v>1486</v>
+      </c>
+      <c r="C511" s="0" t="s">
+        <v>1487</v>
+      </c>
+      <c r="D511" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E511" s="0" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" s="0" t="s">
+        <v>1488</v>
+      </c>
+      <c r="B512" s="0" t="s">
+        <v>844</v>
+      </c>
+      <c r="C512" s="0" t="s">
+        <v>1489</v>
+      </c>
+      <c r="D512" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E512" s="0" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" s="0" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B513" s="0" t="s">
+        <v>1491</v>
+      </c>
+      <c r="C513" s="0" t="s">
+        <v>1492</v>
+      </c>
+      <c r="D513" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E513" s="0" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" s="0" t="s">
+        <v>1494</v>
+      </c>
+      <c r="B514" s="0" t="s">
+        <v>1494</v>
+      </c>
+      <c r="C514" s="0" t="s">
+        <v>1495</v>
+      </c>
+      <c r="D514" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E514" s="0" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" s="0" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B515" s="0" t="s">
+        <v>1497</v>
+      </c>
+      <c r="C515" s="0" t="s">
+        <v>1498</v>
+      </c>
+      <c r="D515" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E515" s="0" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" s="0" t="s">
+        <v>1499</v>
+      </c>
+      <c r="B516" s="0" t="s">
+        <v>1500</v>
+      </c>
+      <c r="C516" s="0" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D516" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E516" s="0" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" s="0" t="s">
+        <v>1502</v>
+      </c>
+      <c r="B517" s="0" t="s">
+        <v>1503</v>
+      </c>
+      <c r="C517" s="0" t="s">
+        <v>1504</v>
+      </c>
+      <c r="D517" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E517" s="0" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" s="0" t="s">
+        <v>1505</v>
+      </c>
+      <c r="B518" s="0" t="s">
+        <v>1505</v>
+      </c>
+      <c r="C518" s="0" t="s">
+        <v>1506</v>
+      </c>
+      <c r="D518" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E518" s="0" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" s="0" t="s">
+        <v>1507</v>
+      </c>
+      <c r="B519" s="0" t="s">
+        <v>1507</v>
+      </c>
+      <c r="C519" s="0" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D519" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E519" s="0" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" s="0" t="s">
+        <v>1509</v>
+      </c>
+      <c r="B520" s="0" t="s">
+        <v>1509</v>
+      </c>
+      <c r="C520" s="0" t="s">
+        <v>1510</v>
+      </c>
+      <c r="D520" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E520" s="0" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" s="0" t="s">
+        <v>1511</v>
+      </c>
+      <c r="B521" s="0" t="s">
+        <v>1511</v>
+      </c>
+      <c r="C521" s="0" t="s">
+        <v>1512</v>
+      </c>
+      <c r="D521" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E521" s="0" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" s="0" t="s">
+        <v>1513</v>
+      </c>
+      <c r="B522" s="0" t="s">
+        <v>1513</v>
+      </c>
+      <c r="C522" s="0" t="s">
+        <v>1514</v>
+      </c>
+      <c r="D522" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E522" s="0" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" s="0" t="s">
+        <v>1515</v>
+      </c>
+      <c r="B523" s="0" t="s">
+        <v>1516</v>
+      </c>
+      <c r="C523" s="0" t="s">
+        <v>1517</v>
+      </c>
+      <c r="D523" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E523" s="0" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" s="0" t="s">
+        <v>1518</v>
+      </c>
+      <c r="B524" s="0" t="s">
+        <v>1519</v>
+      </c>
+      <c r="C524" s="0" t="s">
+        <v>1520</v>
+      </c>
+      <c r="D524" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E524" s="0" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" s="0" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B525" s="0" t="s">
+        <v>1523</v>
+      </c>
+      <c r="C525" s="0" t="s">
+        <v>1524</v>
+      </c>
+      <c r="D525" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E525" s="0" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" s="0" t="s">
+        <v>1525</v>
+      </c>
+      <c r="B526" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="C526" s="0" t="s">
+        <v>1527</v>
+      </c>
+      <c r="D526" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E526" s="0" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" s="0" t="s">
+        <v>1528</v>
+      </c>
+      <c r="B527" s="0" t="s">
+        <v>1529</v>
+      </c>
+      <c r="C527" s="0" t="s">
+        <v>1530</v>
+      </c>
+      <c r="D527" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E527" s="0" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" s="0" t="s">
+        <v>1531</v>
+      </c>
+      <c r="B528" s="0" t="s">
+        <v>1532</v>
+      </c>
+      <c r="C528" s="0" t="s">
+        <v>1533</v>
+      </c>
+      <c r="D528" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E528" s="0" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" s="0" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B529" s="0" t="s">
+        <v>1535</v>
+      </c>
+      <c r="C529" s="0" t="s">
+        <v>1536</v>
+      </c>
+      <c r="D529" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E529" s="0" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" s="0" t="s">
+        <v>1537</v>
+      </c>
+      <c r="B530" s="0" t="s">
+        <v>1538</v>
+      </c>
+      <c r="C530" s="0" t="s">
+        <v>1539</v>
+      </c>
+      <c r="D530" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E530" s="0" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" s="0" t="s">
+        <v>1540</v>
+      </c>
+      <c r="B531" s="0" t="s">
+        <v>1541</v>
+      </c>
+      <c r="C531" s="0" t="s">
+        <v>1542</v>
+      </c>
+      <c r="D531" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E531" s="0" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" s="0" t="s">
+        <v>1543</v>
+      </c>
+      <c r="B532" s="0" t="s">
+        <v>1544</v>
+      </c>
+      <c r="C532" s="0" t="s">
+        <v>1545</v>
+      </c>
+      <c r="D532" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E532" s="0" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" s="0" t="s">
+        <v>1546</v>
+      </c>
+      <c r="B533" s="0" t="s">
+        <v>1547</v>
+      </c>
+      <c r="C533" s="0" t="s">
+        <v>1548</v>
+      </c>
+      <c r="D533" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E533" s="0" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" s="0" t="s">
+        <v>1549</v>
+      </c>
+      <c r="B534" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C534" s="0" t="s">
+        <v>1550</v>
+      </c>
+      <c r="D534" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E534" s="0" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" s="0" t="s">
+        <v>1551</v>
+      </c>
+      <c r="B535" s="0" t="s">
+        <v>1552</v>
+      </c>
+      <c r="C535" s="0" t="s">
+        <v>1553</v>
+      </c>
+      <c r="D535" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E535" s="0" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" s="0" t="s">
+        <v>1554</v>
+      </c>
+      <c r="B536" s="0" t="s">
+        <v>1555</v>
+      </c>
+      <c r="C536" s="0" t="s">
+        <v>1556</v>
+      </c>
+      <c r="D536" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E536" s="0" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" s="0" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B537" s="0" t="s">
+        <v>1558</v>
+      </c>
+      <c r="C537" s="0" t="s">
+        <v>1559</v>
+      </c>
+      <c r="D537" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E537" s="0" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" s="0" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B538" s="0" t="s">
+        <v>1561</v>
+      </c>
+      <c r="C538" s="0" t="s">
+        <v>1562</v>
+      </c>
+      <c r="D538" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E538" s="0" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" s="0" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B539" s="0" t="s">
+        <v>1565</v>
+      </c>
+      <c r="C539" s="0" t="s">
+        <v>1566</v>
+      </c>
+      <c r="D539" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E539" s="0" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" s="0" t="s">
+        <v>1567</v>
+      </c>
+      <c r="B540" s="0" t="s">
+        <v>1567</v>
+      </c>
+      <c r="C540" s="0" t="s">
+        <v>1568</v>
+      </c>
+      <c r="D540" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E540" s="0" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" s="0" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B541" s="0" t="s">
+        <v>1569</v>
+      </c>
+      <c r="C541" s="0" t="s">
+        <v>1570</v>
+      </c>
+      <c r="D541" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E541" s="0" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" s="0" t="s">
+        <v>1571</v>
+      </c>
+      <c r="B542" s="0" t="s">
+        <v>1571</v>
+      </c>
+      <c r="C542" s="0" t="s">
+        <v>1572</v>
+      </c>
+      <c r="D542" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E542" s="0" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" s="0" t="s">
+        <v>1573</v>
+      </c>
+      <c r="B543" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C543" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D543" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E543" s="0" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" s="0" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B544" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C544" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D544" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E544" s="0" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" s="0" t="s">
+        <v>1575</v>
+      </c>
+      <c r="B545" s="0" t="s">
+        <v>1576</v>
+      </c>
+      <c r="C545" s="0" t="s">
+        <v>1577</v>
+      </c>
+      <c r="D545" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E545" s="0" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" s="0" t="s">
+        <v>1578</v>
+      </c>
+      <c r="B546" s="0" t="s">
+        <v>1578</v>
+      </c>
+      <c r="C546" s="0" t="s">
+        <v>1579</v>
+      </c>
+      <c r="D546" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E546" s="0" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" s="0" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B547" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="C547" s="0" t="s">
+        <v>1581</v>
+      </c>
+      <c r="D547" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E547" s="0" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" s="0" t="s">
+        <v>1582</v>
+      </c>
+      <c r="B548" s="0" t="s">
+        <v>1582</v>
+      </c>
+      <c r="C548" s="0" t="s">
+        <v>1583</v>
+      </c>
+      <c r="D548" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E548" s="0" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" s="0" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B549" s="0" t="s">
+        <v>1584</v>
+      </c>
+      <c r="C549" s="0" t="s">
+        <v>1585</v>
+      </c>
+      <c r="D549" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E549" s="0" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" s="0" t="s">
+        <v>1586</v>
+      </c>
+      <c r="B550" s="0" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C550" s="0" t="s">
+        <v>1587</v>
+      </c>
+      <c r="D550" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E550" s="0" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" s="0" t="s">
+        <v>1588</v>
+      </c>
+      <c r="B551" s="0" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C551" s="0" t="s">
+        <v>1589</v>
+      </c>
+      <c r="D551" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E551" s="0" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" s="0" t="s">
+        <v>1590</v>
+      </c>
+      <c r="B552" s="0" t="s">
+        <v>1590</v>
+      </c>
+      <c r="C552" s="0" t="s">
+        <v>1591</v>
+      </c>
+      <c r="D552" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E552" s="0" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" s="0" t="s">
+        <v>1592</v>
+      </c>
+      <c r="B553" s="0" t="s">
+        <v>1592</v>
+      </c>
+      <c r="C553" s="0" t="s">
+        <v>1593</v>
+      </c>
+      <c r="D553" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E553" s="0" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" s="0" t="s">
+        <v>1594</v>
+      </c>
+      <c r="B554" s="0" t="s">
+        <v>1595</v>
+      </c>
+      <c r="C554" s="0" t="s">
+        <v>1596</v>
+      </c>
+      <c r="D554" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E554" s="0" t="s">
+        <v>1563</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UI for AWC exclude abilities
UI for AWC exclude abilities
</commit_message>
<xml_diff>
--- a/Xcom2ClassManager/XComAbilityList.xlsx
+++ b/Xcom2ClassManager/XComAbilityList.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="1597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="1609">
   <si>
     <t>Name</t>
   </si>
@@ -4810,6 +4810,42 @@
   </si>
   <si>
     <t>While Overdrive is active, break through walls and cover when moving.</t>
+  </si>
+  <si>
+    <t>FW_FireMachinePistol</t>
+  </si>
+  <si>
+    <t>Fire Machine Pistol</t>
+  </si>
+  <si>
+    <t>Fire 3 shots at a target with your secondary weapon.</t>
+  </si>
+  <si>
+    <t>Machine Pistol</t>
+  </si>
+  <si>
+    <t>FW_HeavyRounds</t>
+  </si>
+  <si>
+    <t>Heavy Rounds</t>
+  </si>
+  <si>
+    <t>Shots fired by your machine pistol now deal 1 additional damage.</t>
+  </si>
+  <si>
+    <t>FW_MachineSpray</t>
+  </si>
+  <si>
+    <t>Fire 4 shots at a target with your secondary weapon.</t>
+  </si>
+  <si>
+    <t>FW_Yellowjacket</t>
+  </si>
+  <si>
+    <t>Yellowjacket</t>
+  </si>
+  <si>
+    <t>Shots fired by your machine pistol now ignore armor.</t>
   </si>
 </sst>
 </file>
@@ -5152,7 +5188,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G554"/>
+  <dimension ref="A1:G558"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
       <selection activeCell="F76" sqref="F76"/>
@@ -14803,6 +14839,74 @@
       </c>
       <c r="E554" s="0" t="s">
         <v>1563</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" s="0" t="s">
+        <v>1597</v>
+      </c>
+      <c r="B555" s="0" t="s">
+        <v>1598</v>
+      </c>
+      <c r="C555" s="0" t="s">
+        <v>1599</v>
+      </c>
+      <c r="D555" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E555" s="0" t="s">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" s="0" t="s">
+        <v>1601</v>
+      </c>
+      <c r="B556" s="0" t="s">
+        <v>1602</v>
+      </c>
+      <c r="C556" s="0" t="s">
+        <v>1603</v>
+      </c>
+      <c r="D556" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E556" s="0" t="s">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" s="0" t="s">
+        <v>1604</v>
+      </c>
+      <c r="B557" s="0" t="s">
+        <v>1598</v>
+      </c>
+      <c r="C557" s="0" t="s">
+        <v>1605</v>
+      </c>
+      <c r="D557" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E557" s="0" t="s">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" s="0" t="s">
+        <v>1606</v>
+      </c>
+      <c r="B558" s="0" t="s">
+        <v>1607</v>
+      </c>
+      <c r="C558" s="0" t="s">
+        <v>1608</v>
+      </c>
+      <c r="D558" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E558" s="0" t="s">
+        <v>1600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>